<commit_message>
add manual computation of "一步一步地体验梯度下降"
</commit_message>
<xml_diff>
--- a/issues+history/excel/梯度下降法.xlsx.xlsx
+++ b/issues+history/excel/梯度下降法.xlsx.xlsx
@@ -24,7 +24,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <r>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>i</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>z</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>∂</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>∂</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x=2x</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>∂</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>∂</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>y=2y</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
   <si>
     <r>
       <t>x</t>
@@ -44,44 +148,41 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <r>
-      <t>y</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>i</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>位置</t>
-  </si>
-  <si>
-    <t>梯度</t>
-  </si>
-  <si>
-    <t>函数值</t>
-  </si>
-  <si>
-    <t>位移向量</t>
-  </si>
-  <si>
+    <t>梯度下降法</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>点坐标</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>点序号</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>点的位移向量</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>点的偏导数（梯度）</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>点的函数值</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>步长</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>η</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>⊿x=(</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -124,123 +225,139 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>y</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>⊿x</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>⊿y</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>z</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>（例）z=x</t>
-    </r>
-    <r>
-      <rPr>
+      <t>x)*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>η</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>⊿y=(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>∂</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>∂</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>y)*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>η</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>函数</t>
+  </si>
+  <si>
+    <r>
+      <t>z=x</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <vertAlign val="superscript"/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="3"/>
-        <charset val="128"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>2</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="128"/>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>+y</t>
     </r>
     <r>
       <rPr>
+        <b/>
         <vertAlign val="superscript"/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="3"/>
-        <charset val="128"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>2</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="128"/>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>∂</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>z/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>∂</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>η</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>学习率</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>梯度下降法</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -248,10 +365,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="0.000000_ "/>
+    <numFmt numFmtId="177" formatCode="0.000_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,15 +382,6 @@
       <sz val="6"/>
       <name val="宋体"/>
       <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -291,6 +400,82 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -394,7 +579,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -404,17 +589,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -425,16 +622,46 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -717,292 +944,308 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I13"/>
+  <dimension ref="B2:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="9" width="7.7265625" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="14.90625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+    </row>
+    <row r="3" spans="2:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="2" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.8</v>
+    <row r="4" spans="2:9" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="25">
+        <v>0.6</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="2" t="s">
-        <v>6</v>
+      <c r="D6" s="16"/>
+      <c r="E6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="17" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>0</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="14">
         <v>2</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="14">
         <v>3</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="11">
         <f>2*C8</f>
         <v>4</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="11">
         <f>2*D8</f>
         <v>6</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="11">
         <f>-$C4*E8</f>
-        <v>-3.2</v>
-      </c>
-      <c r="H8" s="7">
+        <v>-2.4</v>
+      </c>
+      <c r="H8" s="11">
         <f>-$C4*F8</f>
-        <v>-4.8000000000000007</v>
-      </c>
-      <c r="I8" s="7">
-        <f>C8^2+D8^2</f>
+        <v>-3.5999999999999996</v>
+      </c>
+      <c r="I8" s="14">
+        <f t="shared" ref="I8:I13" si="0">C8^2+D8^2</f>
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>1</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="20">
         <f>C8+G8</f>
-        <v>-1.2000000000000002</v>
-      </c>
-      <c r="D9" s="8">
+        <v>-0.39999999999999991</v>
+      </c>
+      <c r="D9" s="20">
         <f>D8+H8</f>
-        <v>-1.8000000000000007</v>
-      </c>
-      <c r="E9" s="8">
-        <f>2*C9</f>
-        <v>-2.4000000000000004</v>
-      </c>
-      <c r="F9" s="8">
-        <f>2*D9</f>
-        <v>-3.6000000000000014</v>
-      </c>
-      <c r="G9" s="8">
-        <f>-$C$4*E9</f>
-        <v>1.9200000000000004</v>
-      </c>
-      <c r="H9" s="8">
-        <f>-$C$4*F9</f>
-        <v>2.8800000000000012</v>
-      </c>
-      <c r="I9" s="8">
-        <f t="shared" ref="I9:I13" si="0">C9^2+D9^2</f>
-        <v>4.6800000000000033</v>
+        <v>-0.59999999999999964</v>
+      </c>
+      <c r="E9" s="12">
+        <f t="shared" ref="E9:F10" si="1">2*C9</f>
+        <v>-0.79999999999999982</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" si="1"/>
+        <v>-1.1999999999999993</v>
+      </c>
+      <c r="G9" s="12">
+        <f>-$C4*E9</f>
+        <v>0.47999999999999987</v>
+      </c>
+      <c r="H9" s="12">
+        <f>-$C4*F9</f>
+        <v>0.71999999999999953</v>
+      </c>
+      <c r="I9" s="20">
+        <f t="shared" si="0"/>
+        <v>0.51999999999999957</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>2</v>
       </c>
-      <c r="C10" s="8">
-        <f t="shared" ref="C10:C13" si="1">C9+G9</f>
-        <v>0.7200000000000002</v>
-      </c>
-      <c r="D10" s="8">
-        <f t="shared" ref="D10:D13" si="2">D9+H9</f>
-        <v>1.0800000000000005</v>
-      </c>
-      <c r="E10" s="8">
-        <f t="shared" ref="E10:E13" si="3">2*C10</f>
-        <v>1.4400000000000004</v>
-      </c>
-      <c r="F10" s="8">
-        <f>2*D10</f>
-        <v>2.160000000000001</v>
-      </c>
-      <c r="G10" s="8">
-        <f>-$C$4*E10</f>
-        <v>-1.1520000000000004</v>
-      </c>
-      <c r="H10" s="8">
-        <f>-$C$4*F10</f>
-        <v>-1.7280000000000009</v>
-      </c>
-      <c r="I10" s="8">
+      <c r="C10" s="19">
+        <f>C9+G9</f>
+        <v>7.999999999999996E-2</v>
+      </c>
+      <c r="D10" s="19">
+        <f>D9+H9</f>
+        <v>0.11999999999999988</v>
+      </c>
+      <c r="E10" s="12">
+        <f t="shared" si="1"/>
+        <v>0.15999999999999992</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="1"/>
+        <v>0.23999999999999977</v>
+      </c>
+      <c r="G10" s="12">
+        <f>-$C4*E10</f>
+        <v>-9.5999999999999946E-2</v>
+      </c>
+      <c r="H10" s="12">
+        <f>-$C4*F10</f>
+        <v>-0.14399999999999985</v>
+      </c>
+      <c r="I10" s="19">
         <f t="shared" si="0"/>
-        <v>1.6848000000000014</v>
+        <v>2.0799999999999964E-2</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>3</v>
       </c>
-      <c r="C11" s="8">
-        <f t="shared" si="1"/>
-        <v>-0.43200000000000016</v>
-      </c>
-      <c r="D11" s="8">
-        <f t="shared" si="2"/>
-        <v>-0.64800000000000035</v>
-      </c>
-      <c r="E11" s="8">
-        <f t="shared" si="3"/>
-        <v>-0.86400000000000032</v>
-      </c>
-      <c r="F11" s="8">
-        <f t="shared" ref="F11:F13" si="4">2*D11</f>
-        <v>-1.2960000000000007</v>
-      </c>
-      <c r="G11" s="8">
-        <f>-$C$4*E11</f>
-        <v>0.69120000000000026</v>
-      </c>
-      <c r="H11" s="8">
-        <f>-$C$4*F11</f>
-        <v>1.0368000000000006</v>
-      </c>
-      <c r="I11" s="8">
+      <c r="C11" s="18">
+        <f t="shared" ref="C11:C13" si="2">C10+G10</f>
+        <v>-1.5999999999999986E-2</v>
+      </c>
+      <c r="D11" s="18">
+        <f t="shared" ref="D11:D13" si="3">D10+H10</f>
+        <v>-2.3999999999999966E-2</v>
+      </c>
+      <c r="E11" s="12">
+        <f t="shared" ref="E11:E13" si="4">2*C11</f>
+        <v>-3.1999999999999973E-2</v>
+      </c>
+      <c r="F11" s="12">
+        <f t="shared" ref="F11" si="5">2*D11</f>
+        <v>-4.7999999999999932E-2</v>
+      </c>
+      <c r="G11" s="12">
+        <f>-$C4*E11</f>
+        <v>1.9199999999999984E-2</v>
+      </c>
+      <c r="H11" s="12">
+        <f>-$C4*F11</f>
+        <v>2.8799999999999958E-2</v>
+      </c>
+      <c r="I11" s="18">
         <f t="shared" si="0"/>
-        <v>0.60652800000000062</v>
+        <v>8.3199999999999789E-4</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>4</v>
       </c>
-      <c r="C12" s="8">
-        <f t="shared" si="1"/>
-        <v>0.2592000000000001</v>
-      </c>
-      <c r="D12" s="8">
+      <c r="C12" s="17">
         <f t="shared" si="2"/>
-        <v>0.38880000000000026</v>
-      </c>
-      <c r="E12" s="8">
+        <v>3.199999999999998E-3</v>
+      </c>
+      <c r="D12" s="17">
         <f t="shared" si="3"/>
-        <v>0.51840000000000019</v>
-      </c>
-      <c r="F12" s="8">
+        <v>4.7999999999999918E-3</v>
+      </c>
+      <c r="E12" s="12">
         <f t="shared" si="4"/>
-        <v>0.77760000000000051</v>
-      </c>
-      <c r="G12" s="8">
-        <f>-$C$4*E12</f>
-        <v>-0.4147200000000002</v>
-      </c>
-      <c r="H12" s="8">
-        <f>-$C$4*F12</f>
-        <v>-0.62208000000000041</v>
-      </c>
-      <c r="I12" s="8">
+        <v>6.399999999999996E-3</v>
+      </c>
+      <c r="F12" s="12">
+        <f>2*D12</f>
+        <v>9.5999999999999835E-3</v>
+      </c>
+      <c r="G12" s="12">
+        <f>-$C4*E12</f>
+        <v>-3.8399999999999975E-3</v>
+      </c>
+      <c r="H12" s="12">
+        <f>-$C4*F12</f>
+        <v>-5.75999999999999E-3</v>
+      </c>
+      <c r="I12" s="17">
         <f t="shared" si="0"/>
-        <v>0.21835008000000025</v>
+        <v>3.3279999999999912E-5</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>5</v>
       </c>
-      <c r="C13" s="9">
-        <f t="shared" si="1"/>
-        <v>-0.1555200000000001</v>
-      </c>
-      <c r="D13" s="9">
+      <c r="C13" s="21">
         <f t="shared" si="2"/>
-        <v>-0.23328000000000015</v>
-      </c>
-      <c r="E13" s="9">
+        <v>-6.3999999999999951E-4</v>
+      </c>
+      <c r="D13" s="21">
         <f t="shared" si="3"/>
-        <v>-0.31104000000000021</v>
-      </c>
-      <c r="F13" s="9">
+        <v>-9.5999999999999818E-4</v>
+      </c>
+      <c r="E13" s="13">
         <f t="shared" si="4"/>
-        <v>-0.46656000000000031</v>
-      </c>
-      <c r="G13" s="9">
-        <f>-$C$4*E13</f>
-        <v>0.24883200000000016</v>
-      </c>
-      <c r="H13" s="9">
-        <f>-$C$4*F13</f>
-        <v>0.37324800000000025</v>
-      </c>
-      <c r="I13" s="9">
+        <v>-1.279999999999999E-3</v>
+      </c>
+      <c r="F13" s="13">
+        <f>2*D13</f>
+        <v>-1.9199999999999964E-3</v>
+      </c>
+      <c r="G13" s="13">
+        <f>-$C4*E13</f>
+        <v>7.6799999999999937E-4</v>
+      </c>
+      <c r="H13" s="13">
+        <f>-$C4*F13</f>
+        <v>1.1519999999999979E-3</v>
+      </c>
+      <c r="I13" s="21">
         <f t="shared" si="0"/>
-        <v>7.8606028800000102E-2</v>
+        <v>1.3311999999999958E-6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B2:I2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>